<commit_message>
Script creación BBDD (versión completa) #7
BBDD donde se han incluido los UI defauts. No se refleja en el scripts generado automáticamente.
Se ha corregido la documentación de soporte por algún error detectado.
</commit_message>
<xml_diff>
--- a/Documentación Soporte/Etiquetas UI Defaults.xlsx
+++ b/Documentación Soporte/Etiquetas UI Defaults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Documents\UBU\TFG\_Documentos proyecto\Modelado de Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17FE324-4F54-474A-A5D2-9BA4B89DCCE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1A8010-ADA2-4E90-B036-2B8FB10353BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="20700" windowHeight="11140" xr2:uid="{43EB5FC0-7EB3-4F5E-B305-319A8837A03E}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="574">
   <si>
     <t>ATRIBUTOS_PREVISION</t>
   </si>
@@ -1757,6 +1757,9 @@
   </si>
   <si>
     <t>Identificador único de la aplicación presupuestaria de la imputación previsión.</t>
+  </si>
+  <si>
+    <t>Tipo de modificación presupuestaria.</t>
   </si>
 </sst>
 </file>
@@ -2116,7 +2119,7 @@
   <dimension ref="A1:D354"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C361" sqref="C361"/>
+      <selection activeCell="D341" sqref="D341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4787,7 +4790,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>185</v>
       </c>
@@ -4801,7 +4804,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>185</v>
       </c>
@@ -4815,7 +4818,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>185</v>
       </c>
@@ -4829,7 +4832,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>185</v>
       </c>
@@ -6716,7 +6719,7 @@
         <v>419</v>
       </c>
       <c r="D328" t="s">
-        <v>566</v>
+        <v>573</v>
       </c>
     </row>
     <row r="329" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
@@ -6873,7 +6876,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="340" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
         <v>275</v>
       </c>
@@ -6887,7 +6890,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="341" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
         <v>275</v>
       </c>
@@ -7087,7 +7090,7 @@
   <autoFilter ref="A1:D354" xr:uid="{56B75986-C212-42AA-8261-1FFC4D96F05B}">
     <filterColumn colId="0">
       <filters>
-        <filter val="MODELOS"/>
+        <filter val="VINCULANTES"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>